<commit_message>
Fix for calculation on load.
</commit_message>
<xml_diff>
--- a/test/perl_output/demo.xlsx
+++ b/test/perl_output/demo.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Another sheet" sheetId="2" r:id="rId2"/>
     <sheet name="And another" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Features of WriteXLSX</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>http://www.ruby-lang.org/</t>
+  </si>
+  <si>
+    <t>Images</t>
   </si>
   <si>
     <t>Page/printer setup</t>
@@ -143,6 +146,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="republic.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2600325" y="2105025"/>
+          <a:ext cx="1143000" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,14 +559,19 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -528,6 +579,7 @@
     <hyperlink ref="B9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>